<commit_message>
JASM register/Amazon Reg form/Amazon login
</commit_message>
<xml_diff>
--- a/Selenium+Basic_programs/TestData/Raghu.xlsx
+++ b/Selenium+Basic_programs/TestData/Raghu.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raghuveer\eclipse-workspace\BasicProgram_GroTechMinds\Selenium+Basic_programs\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AE4F49-0AC3-4373-9D88-CF475264D63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E8D3FD-83C7-4767-A814-2BC7D20B1EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="Amazon" sheetId="2" r:id="rId2"/>
+    <sheet name="CAccount" sheetId="4" r:id="rId3"/>
+    <sheet name="JASM" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>veer.raghuveer@gmail.com</t>
   </si>
@@ -42,10 +45,49 @@
     <t>manish@01</t>
   </si>
   <si>
-    <t>veer@07</t>
-  </si>
-  <si>
     <t>Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>veer.raghuveer07@gmail.com</t>
+  </si>
+  <si>
+    <t>Amazon$24</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile </t>
+  </si>
+  <si>
+    <t>Raghu</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone No</t>
+  </si>
+  <si>
+    <t>Aadhar</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>veer</t>
+  </si>
+  <si>
+    <t>veer.raghvueer@gmail.com</t>
+  </si>
+  <si>
+    <t>AULPR2343</t>
   </si>
 </sst>
 </file>
@@ -90,9 +132,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -374,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,15 +457,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" s="1">
+        <v>9600850349</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -411,6 +474,11 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -418,7 +486,155 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6853B7C0-29B3-44DB-A320-9EFBDE1086EE}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{E09B7A80-EB87-4D48-88BF-E798CFA28D6F}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{96DFD8EE-4E84-4FA7-8A01-4F0AD8D15D5E}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{D83AE26F-5F43-440F-A019-D400CD11AF6D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F9594B-66B2-40AA-93BC-15978F252B65}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5A7E8351-7120-4646-AC67-3DC4C609B32E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3677C1AA-E240-43B6-8E64-215401DD6861}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1234567890</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{062D17F1-7314-4FD9-849B-49B2BCFB8DB4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87C9054-BA45-45AB-981B-9B84C1AF44D0}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="20.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44556775889</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{729A9C41-47AC-4EC9-8BBE-9DCC34E930B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>